<commit_message>
Update 2021-03-25 Lightbend Platform Due Diligence Report - Included.xlsx
</commit_message>
<xml_diff>
--- a/2021-03-25 Lightbend Platform Due Diligence Report - Included.xlsx
+++ b/2021-03-25 Lightbend Platform Due Diligence Report - Included.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hywel/Documents/GitHub/Included-Licenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D02192-1BC0-B045-961C-C7AA0CE250CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD431EC-16B7-4445-B69A-584F66181A09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21880" yWindow="-28740" windowWidth="49500" windowHeight="27300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29140" yWindow="-28440" windowWidth="49500" windowHeight="27300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="2" r:id="rId1"/>
@@ -11661,13 +11661,13 @@
     <t>Document version 2.8 revised on March 25, 2021 based on the following projects only (note Docker-based commercial products are NOT included in these reports):</t>
   </si>
   <si>
-    <t>**Lightbend Akka Platform**</t>
-  </si>
-  <si>
     <t>In the event of accidental omission, please bring it to our attention by sending email to licenses@lightbend.com</t>
   </si>
   <si>
     <t>Telemetry 2.15.x (formerly known as Cinnamon)</t>
+  </si>
+  <si>
+    <t>Lightbend Akka Platform</t>
   </si>
 </sst>
 </file>
@@ -12093,14 +12093,14 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>3419</v>
+        <v>3421</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -12140,7 +12140,7 @@
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>3420</v>
+        <v>3419</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -12363,7 +12363,7 @@
     <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="5" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>

</xml_diff>